<commit_message>
Added readme and .gitignore
</commit_message>
<xml_diff>
--- a/FplClient/LeagueHistory.xlsx
+++ b/FplClient/LeagueHistory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <x:si>
     <x:t>Game Week</x:t>
   </x:si>
@@ -22,13 +22,16 @@
     <x:t>Lars Christian Eliassen</x:t>
   </x:si>
   <x:si>
+    <x:t>Alma Velagic</x:t>
+  </x:si>
+  <x:si>
     <x:t>Arturo Viveros</x:t>
   </x:si>
   <x:si>
     <x:t>Kjartan Johannesen</x:t>
   </x:si>
   <x:si>
-    <x:t>Alma Velagic</x:t>
+    <x:t>Magnus Ihle</x:t>
   </x:si>
   <x:si>
     <x:t>Kenneth Hansen</x:t>
@@ -37,7 +40,7 @@
     <x:t>Arne Ferkingstad</x:t>
   </x:si>
   <x:si>
-    <x:t>Magnus Ihle</x:t>
+    <x:t>Denis Velagic</x:t>
   </x:si>
   <x:si>
     <x:t>Karl Johan Bore Bjølgerud</x:t>
@@ -46,10 +49,25 @@
     <x:t>Henning Bolstad</x:t>
   </x:si>
   <x:si>
+    <x:t>Hung Huynh</x:t>
+  </x:si>
+  <x:si>
     <x:t>Vidar Andersen</x:t>
   </x:si>
   <x:si>
-    <x:t>Denis Velagic</x:t>
+    <x:t>Vitaly Semenov</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Frode Utvik</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Morten Karlsen</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ryan Phillips</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Geir Ove Drevland</x:t>
   </x:si>
   <x:si>
     <x:t>Jens Vatne Nesse</x:t>
@@ -58,55 +76,43 @@
     <x:t>Sara Svang Rovik</x:t>
   </x:si>
   <x:si>
-    <x:t>Frode Utvik</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Geir Ove Drevland</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ryan Phillips</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hung Huynh</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vitaly Semenov</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Morten Karlsen</x:t>
+    <x:t>Mattias Jacobsson</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Martine Aas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ahsun Taquveem Chohan</x:t>
   </x:si>
   <x:si>
     <x:t>Asmund Haukas</x:t>
   </x:si>
   <x:si>
-    <x:t>Mattias Jacobsson</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Martine Aas</x:t>
+    <x:t>Paal Anders Holmen</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tron Malmø-Lund</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zeus Baba</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kjetil Måge</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mohammad Khattab</x:t>
   </x:si>
   <x:si>
     <x:t>Sara Boberg</x:t>
   </x:si>
   <x:si>
-    <x:t>Ahsun Taquveem Chohan</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kjetil Måge</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zeus Baba</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mohammad Khattab</x:t>
-  </x:si>
-  <x:si>
     <x:t>Staffan Hedstrand</x:t>
   </x:si>
   <x:si>
-    <x:t>Tron Malmø-Lund</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Paal Anders Holmen</x:t>
+    <x:t>Jon Petter hjulstad</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hafiz Rayaan Shahid</x:t>
   </x:si>
   <x:si>
     <x:t>Cato Aune</x:t>
@@ -115,16 +121,13 @@
     <x:t>Rohan Kumar</x:t>
   </x:si>
   <x:si>
-    <x:t>Hafiz Rayaan Shahid</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jon Petter hjulstad</x:t>
-  </x:si>
-  <x:si>
     <x:t>Trond Faksmo</x:t>
   </x:si>
   <x:si>
     <x:t>Anestis Finstad</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Siva Kumar Meejuru</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -499,13 +502,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:AK6"/>
+  <x:dimension ref="A1:AL7"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:37">
+    <x:row r="1" spans="1:38">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -617,112 +620,115 @@
       <x:c r="AK1" s="1" t="s">
         <x:v>36</x:v>
       </x:c>
+      <x:c r="AL1" s="1" t="s">
+        <x:v>37</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:37">
+    <x:row r="2" spans="1:38">
       <x:c r="A2" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="0" t="n">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="C2" s="2" t="n">
+      <x:c r="C2" s="0" t="n">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="D2" s="2" t="n">
         <x:v>99</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="n">
+      <x:c r="E2" s="0" t="n">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="E2" s="0" t="n">
-        <x:v>48</x:v>
-      </x:c>
       <x:c r="F2" s="0" t="n">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="n">
         <x:v>72</x:v>
       </x:c>
-      <x:c r="G2" s="0" t="n">
+      <x:c r="H2" s="0" t="n">
         <x:v>79</x:v>
       </x:c>
-      <x:c r="H2" s="0" t="n">
-        <x:v>60</x:v>
-      </x:c>
       <x:c r="I2" s="0" t="n">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="n">
         <x:v>72</x:v>
       </x:c>
-      <x:c r="J2" s="0" t="n">
+      <x:c r="K2" s="0" t="n">
         <x:v>62</x:v>
       </x:c>
-      <x:c r="K2" s="0" t="n">
+      <x:c r="L2" s="0" t="n">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="M2" s="0" t="n">
         <x:v>61</x:v>
       </x:c>
-      <x:c r="L2" s="0" t="n">
+      <x:c r="N2" s="0" t="n">
         <x:v>57</x:v>
-      </x:c>
-      <x:c r="M2" s="0" t="n">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="N2" s="0" t="n">
-        <x:v>76</x:v>
       </x:c>
       <x:c r="O2" s="0" t="n">
         <x:v>69</x:v>
       </x:c>
       <x:c r="P2" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="Q2" s="0" t="n">
         <x:v>43</x:v>
       </x:c>
       <x:c r="R2" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="S2" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="T2" s="0" t="n">
-        <x:v>62</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="U2" s="0" t="n">
-        <x:v>56</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="V2" s="0" t="n">
         <x:v>64</x:v>
       </x:c>
       <x:c r="W2" s="0" t="n">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="X2" s="0" t="n">
-        <x:v>46</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="Y2" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="Z2" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="AA2" s="0" t="n">
         <x:v>47</x:v>
       </x:c>
       <x:c r="AB2" s="0" t="n">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="AC2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="AC2" s="0" t="n">
+      <x:c r="AD2" s="0" t="n">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="AE2" s="0" t="n">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="AD2" s="0" t="n">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="AE2" s="0" t="n">
-        <x:v>38</x:v>
-      </x:c>
       <x:c r="AF2" s="0" t="n">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="AG2" s="0" t="n">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="AH2" s="0" t="n">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="AG2" s="0" t="n">
+      <x:c r="AI2" s="0" t="n">
         <x:v>20</x:v>
-      </x:c>
-      <x:c r="AH2" s="0" t="n">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="AI2" s="0" t="n">
-        <x:v>33</x:v>
       </x:c>
       <x:c r="AJ2" s="0" t="n">
         <x:v>0</x:v>
@@ -730,112 +736,115 @@
       <x:c r="AK2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AL2" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="3" spans="1:37">
+    <x:row r="3" spans="1:38">
       <x:c r="A3" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="0" t="n">
         <x:v>81</x:v>
       </x:c>
-      <x:c r="C3" s="0" t="n">
+      <x:c r="C3" s="2" t="n">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="n">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="n">
+      <x:c r="E3" s="0" t="n">
         <x:v>71</x:v>
       </x:c>
-      <x:c r="E3" s="2" t="n">
-        <x:v>113</x:v>
-      </x:c>
       <x:c r="F3" s="0" t="n">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="n">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="G3" s="0" t="n">
+      <x:c r="H3" s="0" t="n">
         <x:v>76</x:v>
       </x:c>
-      <x:c r="H3" s="0" t="n">
-        <x:v>67</x:v>
-      </x:c>
       <x:c r="I3" s="0" t="n">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="J3" s="0" t="n">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="J3" s="0" t="n">
+      <x:c r="K3" s="0" t="n">
         <x:v>66</x:v>
       </x:c>
-      <x:c r="K3" s="0" t="n">
+      <x:c r="L3" s="0" t="n">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="M3" s="0" t="n">
         <x:v>81</x:v>
       </x:c>
-      <x:c r="L3" s="0" t="n">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="M3" s="0" t="n">
-        <x:v>86</x:v>
-      </x:c>
       <x:c r="N3" s="0" t="n">
-        <x:v>31</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="O3" s="0" t="n">
         <x:v>53</x:v>
       </x:c>
       <x:c r="P3" s="0" t="n">
-        <x:v>60</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="Q3" s="0" t="n">
         <x:v>61</x:v>
       </x:c>
       <x:c r="R3" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="S3" s="0" t="n">
-        <x:v>82</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="T3" s="0" t="n">
-        <x:v>58</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="U3" s="0" t="n">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="V3" s="0" t="n">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="W3" s="0" t="n">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="X3" s="0" t="n">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="V3" s="0" t="n">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="W3" s="0" t="n">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="X3" s="0" t="n">
-        <x:v>82</x:v>
-      </x:c>
       <x:c r="Y3" s="0" t="n">
-        <x:v>53</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="Z3" s="0" t="n">
-        <x:v>36</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="AA3" s="0" t="n">
         <x:v>53</x:v>
       </x:c>
       <x:c r="AB3" s="0" t="n">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="AC3" s="0" t="n">
         <x:v>71</x:v>
       </x:c>
-      <x:c r="AC3" s="0" t="n">
+      <x:c r="AD3" s="0" t="n">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="AE3" s="0" t="n">
         <x:v>65</x:v>
       </x:c>
-      <x:c r="AD3" s="0" t="n">
-        <x:v>79</x:v>
-      </x:c>
-      <x:c r="AE3" s="0" t="n">
-        <x:v>51</x:v>
-      </x:c>
       <x:c r="AF3" s="0" t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="AG3" s="0" t="n">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="AH3" s="0" t="n">
         <x:v>62</x:v>
       </x:c>
-      <x:c r="AG3" s="0" t="n">
+      <x:c r="AI3" s="0" t="n">
         <x:v>68</x:v>
-      </x:c>
-      <x:c r="AH3" s="0" t="n">
-        <x:v>64</x:v>
-      </x:c>
-      <x:c r="AI3" s="0" t="n">
-        <x:v>39</x:v>
       </x:c>
       <x:c r="AJ3" s="0" t="n">
         <x:v>0</x:v>
@@ -843,8 +852,11 @@
       <x:c r="AK3" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AL3" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="4" spans="1:37">
+    <x:row r="4" spans="1:38">
       <x:c r="A4" s="0" t="n">
         <x:v>3</x:v>
       </x:c>
@@ -852,103 +864,103 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="C4" s="0" t="n">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="n">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="D4" s="0" t="n">
+      <x:c r="E4" s="0" t="n">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="E4" s="0" t="n">
-        <x:v>44</x:v>
-      </x:c>
       <x:c r="F4" s="0" t="n">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="n">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="G4" s="0" t="n">
+      <x:c r="H4" s="0" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="H4" s="0" t="n">
-        <x:v>32</x:v>
-      </x:c>
       <x:c r="I4" s="0" t="n">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="J4" s="0" t="n">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="J4" s="0" t="n">
+      <x:c r="K4" s="0" t="n">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="K4" s="0" t="n">
+      <x:c r="L4" s="2" t="n">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="M4" s="0" t="n">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="L4" s="0" t="n">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="M4" s="0" t="n">
-        <x:v>41</x:v>
-      </x:c>
       <x:c r="N4" s="0" t="n">
-        <x:v>55</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="O4" s="0" t="n">
         <x:v>50</x:v>
       </x:c>
       <x:c r="P4" s="0" t="n">
-        <x:v>41</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="Q4" s="0" t="n">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="R4" s="2" t="n">
-        <x:v>69</x:v>
+      <x:c r="R4" s="0" t="n">
+        <x:v>41</x:v>
       </x:c>
       <x:c r="S4" s="0" t="n">
-        <x:v>22</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="T4" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="U4" s="0" t="n">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="V4" s="0" t="n">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="W4" s="0" t="n">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="X4" s="0" t="n">
         <x:v>34</x:v>
-      </x:c>
-      <x:c r="V4" s="0" t="n">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="W4" s="0" t="n">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="X4" s="0" t="n">
-        <x:v>32</x:v>
       </x:c>
       <x:c r="Y4" s="0" t="n">
         <x:v>49</x:v>
       </x:c>
       <x:c r="Z4" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="AA4" s="0" t="n">
         <x:v>31</x:v>
       </x:c>
       <x:c r="AB4" s="0" t="n">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AC4" s="0" t="n">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="AC4" s="0" t="n">
+      <x:c r="AD4" s="0" t="n">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="AE4" s="0" t="n">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="AD4" s="0" t="n">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="AE4" s="0" t="n">
-        <x:v>49</x:v>
-      </x:c>
       <x:c r="AF4" s="0" t="n">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="AG4" s="0" t="n">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="AH4" s="0" t="n">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="AG4" s="0" t="n">
+      <x:c r="AI4" s="0" t="n">
         <x:v>44</x:v>
-      </x:c>
-      <x:c r="AH4" s="0" t="n">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="AI4" s="0" t="n">
-        <x:v>67</x:v>
       </x:c>
       <x:c r="AJ4" s="0" t="n">
         <x:v>44</x:v>
@@ -956,8 +968,11 @@
       <x:c r="AK4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AL4" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="5" spans="1:37">
+    <x:row r="5" spans="1:38">
       <x:c r="A5" s="0" t="n">
         <x:v>4</x:v>
       </x:c>
@@ -965,103 +980,103 @@
         <x:v>82</x:v>
       </x:c>
       <x:c r="C5" s="0" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="n">
         <x:v>66</x:v>
       </x:c>
-      <x:c r="D5" s="0" t="n">
+      <x:c r="E5" s="0" t="n">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="E5" s="0" t="n">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="F5" s="2" t="n">
+      <x:c r="F5" s="0" t="n">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="G5" s="2" t="n">
         <x:v>88</x:v>
       </x:c>
-      <x:c r="G5" s="0" t="n">
+      <x:c r="H5" s="0" t="n">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="H5" s="0" t="n">
-        <x:v>70</x:v>
-      </x:c>
       <x:c r="I5" s="0" t="n">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="J5" s="0" t="n">
         <x:v>67</x:v>
-      </x:c>
-      <x:c r="J5" s="0" t="n">
-        <x:v>62</x:v>
       </x:c>
       <x:c r="K5" s="0" t="n">
         <x:v>62</x:v>
       </x:c>
       <x:c r="L5" s="0" t="n">
-        <x:v>66</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="M5" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="N5" s="0" t="n">
-        <x:v>65</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="O5" s="0" t="n">
         <x:v>48</x:v>
       </x:c>
       <x:c r="P5" s="0" t="n">
-        <x:v>49</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="Q5" s="0" t="n">
         <x:v>71</x:v>
       </x:c>
       <x:c r="R5" s="0" t="n">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="S5" s="0" t="n">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="T5" s="0" t="n">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="U5" s="0" t="n">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="V5" s="0" t="n">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="W5" s="0" t="n">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="X5" s="0" t="n">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="Y5" s="0" t="n">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="S5" s="0" t="n">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="T5" s="0" t="n">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="U5" s="0" t="n">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="V5" s="0" t="n">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="W5" s="0" t="n">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="X5" s="0" t="n">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="Y5" s="0" t="n">
-        <x:v>34</x:v>
-      </x:c>
       <x:c r="Z5" s="0" t="n">
-        <x:v>50</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="AA5" s="0" t="n">
         <x:v>80</x:v>
       </x:c>
       <x:c r="AB5" s="0" t="n">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AC5" s="0" t="n">
         <x:v>59</x:v>
       </x:c>
-      <x:c r="AC5" s="0" t="n">
+      <x:c r="AD5" s="0" t="n">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="AE5" s="0" t="n">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="AD5" s="0" t="n">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="AE5" s="0" t="n">
+      <x:c r="AF5" s="0" t="n">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="AG5" s="0" t="n">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="AF5" s="0" t="n">
+      <x:c r="AH5" s="0" t="n">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="AG5" s="0" t="n">
+      <x:c r="AI5" s="0" t="n">
         <x:v>44</x:v>
-      </x:c>
-      <x:c r="AH5" s="0" t="n">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="AI5" s="0" t="n">
-        <x:v>22</x:v>
       </x:c>
       <x:c r="AJ5" s="0" t="n">
         <x:v>38</x:v>
@@ -1069,118 +1084,240 @@
       <x:c r="AK5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="AL5" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
-    <x:row r="6" spans="1:37">
+    <x:row r="6" spans="1:38">
       <x:c r="A6" s="0" t="n">
         <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="0" t="n">
         <x:v>81</x:v>
       </x:c>
-      <x:c r="C6" s="2" t="n">
+      <x:c r="C6" s="0" t="n">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="D6" s="2" t="n">
         <x:v>89</x:v>
       </x:c>
-      <x:c r="D6" s="0" t="n">
+      <x:c r="E6" s="0" t="n">
         <x:v>76</x:v>
       </x:c>
-      <x:c r="E6" s="0" t="n">
-        <x:v>67</x:v>
-      </x:c>
       <x:c r="F6" s="0" t="n">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="n">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="G6" s="0" t="n">
+      <x:c r="H6" s="0" t="n">
         <x:v>73</x:v>
       </x:c>
-      <x:c r="H6" s="0" t="n">
-        <x:v>72</x:v>
-      </x:c>
       <x:c r="I6" s="0" t="n">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="J6" s="0" t="n">
         <x:v>63</x:v>
       </x:c>
-      <x:c r="J6" s="0" t="n">
+      <x:c r="K6" s="0" t="n">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="K6" s="0" t="n">
+      <x:c r="L6" s="0" t="n">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="M6" s="0" t="n">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="L6" s="0" t="n">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="M6" s="0" t="n">
-        <x:v>52</x:v>
-      </x:c>
       <x:c r="N6" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="O6" s="0" t="n">
         <x:v>65</x:v>
       </x:c>
       <x:c r="P6" s="0" t="n">
-        <x:v>73</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="Q6" s="0" t="n">
         <x:v>62</x:v>
       </x:c>
       <x:c r="R6" s="0" t="n">
-        <x:v>57</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="S6" s="0" t="n">
-        <x:v>68</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="T6" s="0" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="U6" s="0" t="n">
         <x:v>63</x:v>
       </x:c>
-      <x:c r="U6" s="0" t="n">
+      <x:c r="V6" s="0" t="n">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="W6" s="0" t="n">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="X6" s="0" t="n">
         <x:v>71</x:v>
       </x:c>
-      <x:c r="V6" s="0" t="n">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="W6" s="0" t="n">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="X6" s="0" t="n">
-        <x:v>49</x:v>
-      </x:c>
       <x:c r="Y6" s="0" t="n">
-        <x:v>61</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="Z6" s="0" t="n">
-        <x:v>51</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="AA6" s="0" t="n">
         <x:v>43</x:v>
       </x:c>
       <x:c r="AB6" s="0" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AC6" s="0" t="n">
         <x:v>65</x:v>
       </x:c>
-      <x:c r="AC6" s="0" t="n">
+      <x:c r="AD6" s="0" t="n">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AE6" s="0" t="n">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="AD6" s="0" t="n">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="AE6" s="0" t="n">
-        <x:v>48</x:v>
-      </x:c>
       <x:c r="AF6" s="0" t="n">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="AG6" s="0" t="n">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AH6" s="0" t="n">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="AG6" s="0" t="n">
+      <x:c r="AI6" s="0" t="n">
         <x:v>22</x:v>
-      </x:c>
-      <x:c r="AH6" s="0" t="n">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="AI6" s="0" t="n">
-        <x:v>27</x:v>
       </x:c>
       <x:c r="AJ6" s="0" t="n">
         <x:v>55</x:v>
       </x:c>
       <x:c r="AK6" s="0" t="n">
         <x:v>73</x:v>
+      </x:c>
+      <x:c r="AL6" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:38">
+      <x:c r="A7" s="0" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="n">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C7" s="2" t="n">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="n">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="n">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="n">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="n">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="H7" s="0" t="n">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="I7" s="0" t="n">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="J7" s="0" t="n">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="K7" s="0" t="n">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="L7" s="0" t="n">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="M7" s="0" t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="N7" s="0" t="n">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="O7" s="0" t="n">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="P7" s="0" t="n">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="Q7" s="0" t="n">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="R7" s="0" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="S7" s="0" t="n">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="T7" s="0" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="U7" s="0" t="n">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="V7" s="0" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="W7" s="0" t="n">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="X7" s="0" t="n">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="Y7" s="0" t="n">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="Z7" s="0" t="n">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="AA7" s="0" t="n">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AB7" s="0" t="n">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="AC7" s="0" t="n">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="AD7" s="0" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="AE7" s="0" t="n">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="AF7" s="0" t="n">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="AG7" s="0" t="n">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AH7" s="0" t="n">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="AI7" s="0" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="AJ7" s="0" t="n">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="AK7" s="0" t="n">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="AL7" s="0" t="n">
+        <x:v>35</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>